<commit_message>
gotta fix that insert script to db, added angular app
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -483,12 +483,6 @@
     <t>It's Ice</t>
   </si>
   <si>
-    <t>2016 -&gt;</t>
-  </si>
-  <si>
-    <t>2018-&gt;</t>
-  </si>
-  <si>
     <t>No Men In No Man's Land </t>
   </si>
   <si>
@@ -726,12 +720,6 @@
     <t>Poor Heart </t>
   </si>
   <si>
-    <t>Points</t>
-  </si>
-  <si>
-    <t>Song</t>
-  </si>
-  <si>
     <t xml:space="preserve">Meat </t>
   </si>
   <si>
@@ -757,6 +745,18 @@
   </si>
   <si>
     <t xml:space="preserve">Running tally for all of summer tour </t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>plays_since_2016</t>
+  </si>
+  <si>
+    <t>plays_since_2018</t>
   </si>
 </sst>
 </file>
@@ -1171,36 +1171,37 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+      <selection pane="topRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>150</v>
+        <v>240</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>151</v>
+        <v>241</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2" s="3">
         <v>29</v>
@@ -1218,7 +1219,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B3" s="3">
         <v>29</v>
@@ -1254,7 +1255,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B5" s="3">
         <v>28</v>
@@ -1272,7 +1273,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" s="3">
         <v>27</v>
@@ -1290,7 +1291,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3">
         <v>26</v>
@@ -1308,7 +1309,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B8" s="3">
         <v>27</v>
@@ -1326,7 +1327,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B9" s="3">
         <v>25</v>
@@ -1380,7 +1381,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B12" s="3">
         <v>24</v>
@@ -1398,7 +1399,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B13" s="3">
         <v>25</v>
@@ -1416,7 +1417,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B14" s="3">
         <v>25</v>
@@ -1434,7 +1435,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B15" s="3">
         <v>23</v>
@@ -1452,7 +1453,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16" s="3">
         <v>23</v>
@@ -1470,7 +1471,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B17" s="3">
         <v>23</v>
@@ -1488,7 +1489,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B18" s="3">
         <v>23</v>
@@ -1524,7 +1525,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20" s="3">
         <v>23</v>
@@ -1542,7 +1543,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B21" s="3">
         <v>24</v>
@@ -1560,7 +1561,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B22" s="3">
         <v>22</v>
@@ -1578,7 +1579,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="3">
         <v>23</v>
@@ -1596,7 +1597,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B24" s="3">
         <v>22</v>
@@ -1614,7 +1615,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B25" s="3">
         <v>22</v>
@@ -1632,7 +1633,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B26" s="3">
         <v>21</v>
@@ -1650,7 +1651,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B27" s="3">
         <v>21</v>
@@ -1668,7 +1669,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B28" s="3">
         <v>21</v>
@@ -1686,7 +1687,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B29" s="3">
         <v>20</v>
@@ -1704,7 +1705,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B30" s="3">
         <v>20</v>
@@ -1722,7 +1723,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B31" s="3">
         <v>21</v>
@@ -1740,7 +1741,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B32" s="3">
         <v>15</v>
@@ -1776,7 +1777,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B34" s="3">
         <v>19</v>
@@ -1794,7 +1795,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B35" s="3">
         <v>19</v>
@@ -1866,7 +1867,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B39" s="3">
         <v>15</v>
@@ -1884,7 +1885,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B40" s="3">
         <v>17</v>
@@ -1920,7 +1921,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B42" s="3">
         <v>16</v>
@@ -1956,7 +1957,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B44" s="3">
         <v>16</v>
@@ -1974,7 +1975,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B45" s="3">
         <v>16</v>
@@ -2010,7 +2011,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B47" s="3">
         <v>15</v>
@@ -2046,7 +2047,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B49" s="4">
         <v>13</v>
@@ -2100,7 +2101,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B52" s="4">
         <v>14</v>
@@ -2118,7 +2119,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B53" s="4">
         <v>9</v>
@@ -2136,7 +2137,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B54" s="4">
         <v>13</v>
@@ -2154,7 +2155,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B55" s="4">
         <v>14</v>
@@ -2172,7 +2173,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B56" s="4">
         <v>15</v>
@@ -2190,7 +2191,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B57" s="4">
         <v>13</v>
@@ -2208,7 +2209,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B58" s="4">
         <v>13</v>
@@ -2226,7 +2227,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B59" s="4">
         <v>13</v>
@@ -2244,7 +2245,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B60" s="4">
         <v>13</v>
@@ -2262,7 +2263,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B61" s="4">
         <v>13</v>
@@ -2280,7 +2281,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B62" s="4">
         <v>14</v>
@@ -2298,7 +2299,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B63" s="4">
         <v>11</v>
@@ -2334,7 +2335,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B65" s="4">
         <v>12</v>
@@ -2352,7 +2353,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B66" s="4">
         <v>12</v>
@@ -2388,7 +2389,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B68" s="4">
         <v>12</v>
@@ -2424,7 +2425,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B70" s="4">
         <v>12</v>
@@ -2442,7 +2443,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B71" s="4">
         <v>13</v>
@@ -2478,7 +2479,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B73" s="4">
         <v>8</v>
@@ -2496,7 +2497,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B74" s="4">
         <v>11</v>
@@ -2514,7 +2515,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B75" s="4">
         <v>12</v>
@@ -2532,7 +2533,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B76" s="4">
         <v>12</v>
@@ -2550,7 +2551,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B77" s="4">
         <v>13</v>
@@ -2568,7 +2569,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B78" s="4">
         <v>9</v>
@@ -2604,7 +2605,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B80" s="4">
         <v>10</v>
@@ -2640,7 +2641,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B82" s="4">
         <v>11</v>
@@ -2658,7 +2659,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B83" s="4">
         <v>11</v>
@@ -2694,7 +2695,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B85" s="4">
         <v>11</v>
@@ -2712,7 +2713,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B86" s="4">
         <v>12</v>
@@ -2730,7 +2731,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B87" s="4">
         <v>12</v>
@@ -2766,7 +2767,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B89" s="4">
         <v>9</v>
@@ -2802,7 +2803,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B91" s="4">
         <v>11</v>
@@ -2820,7 +2821,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B92" s="4">
         <v>11</v>
@@ -2838,7 +2839,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B93" s="4">
         <v>8</v>
@@ -2874,7 +2875,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B95" s="4">
         <v>9</v>
@@ -2892,7 +2893,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B96" s="4">
         <v>9</v>
@@ -2910,7 +2911,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B97" s="4">
         <v>9</v>
@@ -2928,7 +2929,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B98" s="4">
         <v>9</v>
@@ -2946,7 +2947,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B99" s="4">
         <v>9</v>
@@ -2982,7 +2983,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B101" s="4">
         <v>9</v>
@@ -3000,7 +3001,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B102" s="4">
         <v>10</v>
@@ -3162,7 +3163,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B111" s="4">
         <v>9</v>
@@ -3360,7 +3361,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B122" s="11">
         <v>5</v>
@@ -4096,7 +4097,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B163" s="5"/>
       <c r="C163" s="5">
@@ -4112,7 +4113,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B164" s="5"/>
       <c r="C164" s="5">
@@ -5222,37 +5223,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>